<commit_message>
corrected loglikelhood descirption in general info files, closes #7
</commit_message>
<xml_diff>
--- a/Benchmark-Models/Becker_Science2010/General_info.xlsx
+++ b/Benchmark-Models/Becker_Science2010/General_info.xlsx
@@ -40,7 +40,7 @@
     <t xml:space="preserve">Errors are assumed as additive Gaussian errors</t>
   </si>
   <si>
-    <t xml:space="preserve">Log-likelihood value of the model is </t>
+    <t xml:space="preserve">2*Log-likelihood value of the model is </t>
   </si>
   <si>
     <t xml:space="preserve">Chi2 value of the model is </t>
@@ -374,7 +374,7 @@
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>